<commit_message>
End of week commit
Updated end of week commit
</commit_message>
<xml_diff>
--- a/DEFRA Migrations/Assets/ConfigurationOptions.xlsx
+++ b/DEFRA Migrations/Assets/ConfigurationOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra-my.sharepoint.com/personal/david_adams_defra_gov_uk/Documents/UiPath/DEFRA-Migrations/DEFRA Migrations/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{88BC5AC4-1376-4517-A70C-A8CD162177D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E6970CA-B607-423A-AA6F-A0757034D984}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{88BC5AC4-1376-4517-A70C-A8CD162177D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BF1AC0B-711B-46F9-9ADF-EE974355EFD1}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{EA615094-B4E9-417A-8393-1C90709E7C7A}"/>
   </bookViews>
@@ -143,10 +143,10 @@
     <t>https://defra.sharepoint.com/sites/Community290</t>
   </si>
   <si>
-    <t>The target destination document library. Not used for Network Drive migrations where the queue item contains this meta data</t>
-  </si>
-  <si>
-    <t>The target destination SharePoint site. Not used for Network Drive migrations where the queue item contains this meta data</t>
+    <t>The target destination document library. Not used for Network Drive migrations (which uses the queue item meta data for this)</t>
+  </si>
+  <si>
+    <t>The target destination SharePoint site. Not used for Network Drive migrations (which uses the queue item meta data for this)</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
End of week check in
End of week check in
</commit_message>
<xml_diff>
--- a/DEFRA Migrations/Assets/ConfigurationOptions.xlsx
+++ b/DEFRA Migrations/Assets/ConfigurationOptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra-my.sharepoint.com/personal/david_adams_defra_gov_uk/Documents/UiPath/DEFRA-Migrations/DEFRA Migrations/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{88BC5AC4-1376-4517-A70C-A8CD162177D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BF1AC0B-711B-46F9-9ADF-EE974355EFD1}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{88BC5AC4-1376-4517-A70C-A8CD162177D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08EC82C5-D341-4A26-A216-0BFE4D4CBDFF}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{EA615094-B4E9-417A-8393-1C90709E7C7A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Configuration Options</t>
   </si>
@@ -62,9 +62,6 @@
     <t>MigrationInProgressAction</t>
   </si>
   <si>
-    <t>What action should the robot take to the current file it is migrating. Options are either MoveToInProgress (moves to a different folder before migrating) or NoMove to keep in present location</t>
-  </si>
-  <si>
     <t>NoAction</t>
   </si>
   <si>
@@ -98,18 +95,12 @@
     <t>MigrationSourceFileCleanUpCopyLocation</t>
   </si>
   <si>
-    <t>The location to copy the source file to during file clean up operations. Only applies when MigrationSourceFileCleanUpAction is set to CopyToCompleted</t>
-  </si>
-  <si>
     <t>C:\Users\x956633\Downloads\Copy\</t>
   </si>
   <si>
     <t>MigrationSourceFileCleanUpMoveLocation</t>
   </si>
   <si>
-    <t>The location to move the source file to during file clean up operations. Only applies when MigrationSourceFileCleanUpAction is set to MoveToCompleted</t>
-  </si>
-  <si>
     <t>C:\Users\x956633\Downloads\Move\</t>
   </si>
   <si>
@@ -147,6 +138,24 @@
   </si>
   <si>
     <t>The target destination SharePoint site. Not used for Network Drive migrations (which uses the queue item meta data for this)</t>
+  </si>
+  <si>
+    <t>The location to move the source file to during file clean up operations. Only applies when MigrationSourceFileCleanUpAction is set to MoveToCompleted. Can use {0} in the path to insert the existing folder structure (ignoring the network drive it is on).</t>
+  </si>
+  <si>
+    <t>The location to copy the source file to during file clean up operations. Only applies when MigrationSourceFileCleanUpAction is set to CopyToCompleted. Can use {0} in the path to insert the existing folder structure (ignoring the network drive it is on).</t>
+  </si>
+  <si>
+    <t>Rename - Underscore Increment</t>
+  </si>
+  <si>
+    <t>If a file with the same name exists in the same location on the Target site, what action should be taken? Options are: Overwrite, Rename - Underscore Increment</t>
+  </si>
+  <si>
+    <t>TargetFileExistsAction</t>
+  </si>
+  <si>
+    <t>What action should the robot take to the current file it is migrating. Options are either Move To In Progress (moves to a different folder before migrating) or No Action to keep in present location</t>
   </si>
 </sst>
 </file>
@@ -508,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34F8CB5-BA69-4816-90C3-C75866F95961}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -539,13 +548,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -564,98 +573,109 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>